<commit_message>
Edit new date and expect result
</commit_message>
<xml_diff>
--- a/663380019-2_Lab4.xlsx
+++ b/663380019-2_Lab4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\QA_Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D0677D-5889-4335-9C31-DF78141C3FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFDFE30-B5ED-4FE1-846A-3893CD6AF9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{2D3B1ECF-CE0B-884D-A6E2-5EDB198A06FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{2D3B1ECF-CE0B-884D-A6E2-5EDB198A06FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="116">
   <si>
     <t>Test Case Design and Test Results</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Gold</t>
-  </si>
-  <si>
     <t>Silver</t>
   </si>
   <si>
@@ -305,37 +302,174 @@
     <t>ปวริศ</t>
   </si>
   <si>
-    <t>Assign</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>คำนวณ Rank ของผู้ใช้งานไม่ถูกต้องตามที่ควรจะเป็น</t>
-  </si>
-  <si>
     <t>DF02</t>
   </si>
   <si>
     <t>Invalid input</t>
   </si>
   <si>
-    <t>มี Input บางตัวที่ไม่ควรใส่เข้าไปในระบบได้แต่ก็ยังใส่ได้</t>
-  </si>
-  <si>
     <t>663380019-2</t>
+  </si>
+  <si>
+    <t>Defect ID</t>
+  </si>
+  <si>
+    <t>DF03</t>
+  </si>
+  <si>
+    <t>DF04</t>
+  </si>
+  <si>
+    <t>DF05</t>
+  </si>
+  <si>
+    <t>DF06</t>
+  </si>
+  <si>
+    <t>DF07</t>
+  </si>
+  <si>
+    <t>DF08</t>
+  </si>
+  <si>
+    <t>DF09</t>
+  </si>
+  <si>
+    <t>DF10</t>
+  </si>
+  <si>
+    <t>DF11</t>
+  </si>
+  <si>
+    <t>DF12</t>
+  </si>
+  <si>
+    <t>DF13</t>
+  </si>
+  <si>
+    <t>DF14</t>
+  </si>
+  <si>
+    <t>DF15</t>
+  </si>
+  <si>
+    <t>DF16</t>
+  </si>
+  <si>
+    <t>DF17</t>
+  </si>
+  <si>
+    <t>DF18</t>
+  </si>
+  <si>
+    <t>DF19</t>
+  </si>
+  <si>
+    <t>DF20</t>
+  </si>
+  <si>
+    <t>DF21</t>
+  </si>
+  <si>
+    <t>DF22</t>
+  </si>
+  <si>
+    <t>คำนวณ Rank ของผู้ใช้งานผิดจาก Standard เป็น Silver</t>
+  </si>
+  <si>
+    <t>คำนวณ Rank ของผู้ใช้งานผิดจาก Silver เป็น Standard</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ไม่ควรใส่ค่ายอดซื้อรวมที่มีค่าเป็น </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunPSK"/>
+        <family val="2"/>
+        <charset val="222"/>
+      </rPr>
+      <t xml:space="preserve">-1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunIT๙"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ได้ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ไม่ควรใส่ค่าจำนวนครั้งที่มาใช้บริการที่มีค่าเป็น </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunPSK"/>
+        <family val="2"/>
+        <charset val="222"/>
+      </rPr>
+      <t xml:space="preserve">-1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunIT๙"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ได้ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ไม่ควรใส่ค่าจำนวนแต้มสะสมที่มีค่าเป็น </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunPSK"/>
+        <family val="2"/>
+        <charset val="222"/>
+      </rPr>
+      <t xml:space="preserve">-1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunIT๙"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ได้ </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -437,6 +571,14 @@
       <color theme="1"/>
       <name val="TH SarabunIT๙"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+      <charset val="222"/>
     </font>
   </fonts>
   <fills count="7">
@@ -575,160 +717,164 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal 3 4" xfId="1" xr:uid="{DD4AD2A2-321B-5F4E-AAE1-B5C53296010C}"/>
     <cellStyle name="Normal_ftest" xfId="2" xr:uid="{2E60872E-C109-5D40-AEB9-649A4B5FF349}"/>
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
     <cellStyle name="ปกติ 2" xfId="4" xr:uid="{DFF96B33-81E0-4AF9-AC7D-AB40DF5E4497}"/>
+    <cellStyle name="ปกติ 3" xfId="5" xr:uid="{410D0A69-95F4-4934-81D7-677054E6A60D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1062,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CE7BA3-0BEF-0C45-955A-B350FDBEC636}">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="27" x14ac:dyDescent="0.75"/>
@@ -1127,10 +1273,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -1156,11 +1302,11 @@
       <c r="B6" s="3">
         <v>32</v>
       </c>
-      <c r="C6" s="49">
-        <v>11</v>
-      </c>
-      <c r="D6" s="50">
-        <v>21</v>
+      <c r="C6" s="27">
+        <v>10</v>
+      </c>
+      <c r="D6" s="28">
+        <v>22</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -1177,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEE3D1E-0814-D34A-9C7B-86FDE5AD12C8}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="27" x14ac:dyDescent="0.75"/>
@@ -1197,29 +1343,29 @@
     <col min="14" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="42"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="G2" s="4"/>
       <c r="J2" s="3" t="s">
         <v>10</v>
@@ -1233,23 +1379,23 @@
       <c r="M2" s="3">
         <v>0</v>
       </c>
-      <c r="N2" s="42"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>9</v>
@@ -1263,18 +1409,18 @@
       <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="N3" s="42"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1286,25 +1432,25 @@
         <v>50000</v>
       </c>
       <c r="L4" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M4" s="3">
         <v>500</v>
       </c>
-      <c r="N4" s="42"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="25">
         <v>244182</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1314,14 +1460,14 @@
         <v>99999</v>
       </c>
       <c r="L5" s="3">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M5" s="3">
         <v>999</v>
       </c>
-      <c r="N5" s="42"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="J6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1329,34 +1475,36 @@
         <v>100000</v>
       </c>
       <c r="L6" s="3">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="M6" s="3">
         <v>1000</v>
       </c>
-      <c r="N6" s="43"/>
-    </row>
-    <row r="7" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="40" t="s">
+    </row>
+    <row r="7" spans="1:14" ht="25.05" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="40" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="40" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A8" s="41"/>
+      <c r="H7" s="50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A8" s="39"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1366,317 +1514,347 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="39"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="43"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="49"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="44">
         <v>0</v>
       </c>
-      <c r="C9" s="32">
-        <v>4</v>
-      </c>
-      <c r="D9" s="32">
+      <c r="C9" s="44">
+        <v>15</v>
+      </c>
+      <c r="D9" s="44">
         <v>500</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E9" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="44">
         <v>1</v>
       </c>
-      <c r="C10" s="32">
-        <v>4</v>
-      </c>
-      <c r="D10" s="32">
+      <c r="C10" s="44">
+        <v>15</v>
+      </c>
+      <c r="D10" s="44">
         <v>500</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="44">
         <v>50000</v>
       </c>
-      <c r="C11" s="32">
-        <v>4</v>
-      </c>
-      <c r="D11" s="32">
+      <c r="C11" s="44">
+        <v>15</v>
+      </c>
+      <c r="D11" s="44">
         <v>500</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="G11" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="44">
         <v>99999</v>
       </c>
-      <c r="C12" s="32">
-        <v>4</v>
-      </c>
-      <c r="D12" s="32">
+      <c r="C12" s="44">
+        <v>15</v>
+      </c>
+      <c r="D12" s="44">
         <v>500</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="G12" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="44">
         <v>100000</v>
       </c>
-      <c r="C13" s="32">
-        <v>4</v>
-      </c>
-      <c r="D13" s="32">
+      <c r="C13" s="44">
+        <v>15</v>
+      </c>
+      <c r="D13" s="44">
         <v>500</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="G13" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="44">
         <v>50000</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="44">
         <v>0</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="44">
         <v>500</v>
       </c>
-      <c r="E14" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E14" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="44">
         <v>50000</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="44">
         <v>1</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="44">
         <v>500</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E15" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="44">
         <v>50000</v>
       </c>
-      <c r="C16" s="32">
-        <v>6</v>
-      </c>
-      <c r="D16" s="32">
+      <c r="C16" s="44">
+        <v>29</v>
+      </c>
+      <c r="D16" s="44">
         <v>500</v>
       </c>
-      <c r="E16" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="E16" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="44">
         <v>50000</v>
       </c>
-      <c r="C17" s="32">
-        <v>7</v>
-      </c>
-      <c r="D17" s="32">
+      <c r="C17" s="44">
+        <v>30</v>
+      </c>
+      <c r="D17" s="44">
         <v>500</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="E17" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="44">
         <v>50000</v>
       </c>
-      <c r="C18" s="32">
-        <v>4</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="44">
+        <v>15</v>
+      </c>
+      <c r="D18" s="44">
         <v>0</v>
       </c>
-      <c r="E18" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="E18" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="44">
         <v>50000</v>
       </c>
-      <c r="C19" s="32">
-        <v>4</v>
-      </c>
-      <c r="D19" s="32">
+      <c r="C19" s="44">
+        <v>15</v>
+      </c>
+      <c r="D19" s="44">
         <v>1</v>
       </c>
-      <c r="E19" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="E19" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="44">
         <v>50000</v>
       </c>
-      <c r="C20" s="32">
-        <v>4</v>
-      </c>
-      <c r="D20" s="32">
+      <c r="C20" s="44">
+        <v>15</v>
+      </c>
+      <c r="D20" s="44">
         <v>999</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G20" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="44">
         <v>50000</v>
       </c>
-      <c r="C21" s="32">
-        <v>4</v>
-      </c>
-      <c r="D21" s="32">
+      <c r="C21" s="44">
+        <v>15</v>
+      </c>
+      <c r="D21" s="44">
         <v>1000</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>83</v>
+      <c r="G21" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B3:E3"/>
@@ -1687,7 +1865,7 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A7:A8"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1696,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A52C6A-99BA-484C-B915-27B6FC4D32AF}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="27" x14ac:dyDescent="0.75"/>
@@ -1715,26 +1893,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="42"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="G2" s="4"/>
@@ -1750,23 +1928,23 @@
       <c r="M2" s="3">
         <v>-1</v>
       </c>
-      <c r="N2" s="42"/>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>10</v>
@@ -1780,18 +1958,18 @@
       <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="N3" s="42"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1808,20 +1986,20 @@
       <c r="M4" s="3">
         <v>1</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="25">
         <v>244183</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1831,12 +2009,12 @@
         <v>50000</v>
       </c>
       <c r="L5" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M5" s="3">
         <v>500</v>
       </c>
-      <c r="N5" s="42"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="J6" s="3" t="s">
@@ -1846,30 +2024,33 @@
         <v>99999</v>
       </c>
       <c r="L6" s="3">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M6" s="3">
         <v>999</v>
       </c>
-      <c r="N6" s="42"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="25.05" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="43" t="s">
         <v>16</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>90</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>6</v>
@@ -1878,15 +2059,14 @@
         <v>100000</v>
       </c>
       <c r="L7" s="3">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="M7" s="3">
         <v>1000</v>
       </c>
-      <c r="N7" s="43"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A8" s="27"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1896,9 +2076,10 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="49"/>
       <c r="J8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1906,453 +2087,502 @@
         <v>100001</v>
       </c>
       <c r="L8" s="3">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="M8" s="3">
         <v>1001</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="18">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="18">
+        <v>15</v>
+      </c>
+      <c r="D9" s="18">
+        <v>500</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="19">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>15</v>
+      </c>
+      <c r="D10" s="19">
+        <v>500</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B11" s="19">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19">
+        <v>500</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C12" s="18">
+        <v>15</v>
+      </c>
+      <c r="D12" s="19">
+        <v>500</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="19">
+        <v>99999</v>
+      </c>
+      <c r="C13" s="18">
+        <v>15</v>
+      </c>
+      <c r="D13" s="19">
+        <v>500</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="19">
+        <v>100000</v>
+      </c>
+      <c r="C14" s="18">
+        <v>15</v>
+      </c>
+      <c r="D14" s="19">
+        <v>500</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="19">
+        <v>100001</v>
+      </c>
+      <c r="C15" s="18">
+        <v>15</v>
+      </c>
+      <c r="D15" s="19">
+        <v>500</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A16" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C16" s="19">
         <v>-1</v>
       </c>
-      <c r="C9" s="30">
-        <v>4</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="D16" s="19">
         <v>500</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E16" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="36" t="s">
+      <c r="F16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A17" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19">
+        <v>500</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="48" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A10" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="31">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A18" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C18" s="19">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19">
+        <v>500</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C19" s="19">
+        <v>29</v>
+      </c>
+      <c r="D19" s="19">
+        <v>500</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C20" s="19">
+        <v>30</v>
+      </c>
+      <c r="D20" s="19">
+        <v>500</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C21" s="19">
+        <v>31</v>
+      </c>
+      <c r="D21" s="19">
+        <v>500</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A22" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C22" s="19">
+        <v>15</v>
+      </c>
+      <c r="D22" s="19">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A23" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C23" s="19">
+        <v>15</v>
+      </c>
+      <c r="D23" s="19">
         <v>0</v>
       </c>
-      <c r="C10" s="31">
-        <v>4</v>
-      </c>
-      <c r="D10" s="31">
-        <v>500</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A11" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="31">
+      <c r="E23" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A24" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C24" s="19">
+        <v>15</v>
+      </c>
+      <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="C11" s="31">
-        <v>4</v>
-      </c>
-      <c r="D11" s="31">
-        <v>500</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A12" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="31">
+      <c r="E24" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A25" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="19">
         <v>50000</v>
       </c>
-      <c r="C12" s="31">
-        <v>4</v>
-      </c>
-      <c r="D12" s="31">
-        <v>500</v>
-      </c>
-      <c r="E12" s="31" t="s">
+      <c r="C25" s="19">
+        <v>15</v>
+      </c>
+      <c r="D25" s="19">
+        <v>999</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A13" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="31">
-        <v>99999</v>
-      </c>
-      <c r="C13" s="31">
-        <v>4</v>
-      </c>
-      <c r="D13" s="31">
-        <v>500</v>
-      </c>
-      <c r="E13" s="31" t="s">
+      <c r="G25" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C26" s="19">
+        <v>15</v>
+      </c>
+      <c r="D26" s="19">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A14" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="31">
-        <v>100000</v>
-      </c>
-      <c r="C14" s="31">
-        <v>4</v>
-      </c>
-      <c r="D14" s="31">
-        <v>500</v>
-      </c>
-      <c r="E14" s="31" t="s">
+      <c r="G26" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A27" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="19">
+        <v>50000</v>
+      </c>
+      <c r="C27" s="19">
+        <v>15</v>
+      </c>
+      <c r="D27" s="19">
+        <v>1001</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A15" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="31">
-        <v>100001</v>
-      </c>
-      <c r="C15" s="31">
-        <v>4</v>
-      </c>
-      <c r="D15" s="31">
-        <v>500</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A16" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C16" s="31">
-        <v>-1</v>
-      </c>
-      <c r="D16" s="31">
-        <v>500</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A17" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C17" s="31">
-        <v>0</v>
-      </c>
-      <c r="D17" s="31">
-        <v>500</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A18" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C18" s="31">
-        <v>1</v>
-      </c>
-      <c r="D18" s="31">
-        <v>500</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C19" s="31">
-        <v>6</v>
-      </c>
-      <c r="D19" s="31">
-        <v>500</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A20" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C20" s="31">
-        <v>7</v>
-      </c>
-      <c r="D20" s="31">
-        <v>500</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A21" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C21" s="31">
-        <v>8</v>
-      </c>
-      <c r="D21" s="31">
-        <v>500</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A22" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C22" s="31">
-        <v>4</v>
-      </c>
-      <c r="D22" s="31">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C23" s="31">
-        <v>4</v>
-      </c>
-      <c r="D23" s="31">
-        <v>0</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A24" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C24" s="31">
-        <v>4</v>
-      </c>
-      <c r="D24" s="31">
-        <v>1</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A25" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C25" s="31">
-        <v>4</v>
-      </c>
-      <c r="D25" s="31">
-        <v>999</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A26" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="31">
-        <v>50000</v>
-      </c>
-      <c r="C26" s="31">
-        <v>4</v>
-      </c>
-      <c r="D26" s="31">
-        <v>1000</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A27" s="29" t="s">
+      <c r="G27" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="31">
-        <v>5000</v>
-      </c>
-      <c r="C27" s="31">
-        <v>4</v>
-      </c>
-      <c r="D27" s="31">
-        <v>1001</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>84</v>
+      <c r="H27" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
@@ -2363,17 +2593,17 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8068CBD9-38BE-794D-AE4F-17FC500CF117}">
-  <dimension ref="A2:K4"/>
+  <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="27" x14ac:dyDescent="0.75"/>
@@ -2421,32 +2651,28 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A3" s="45">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="47">
-        <v>244182</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46" t="s">
-        <v>90</v>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.75">
@@ -2454,31 +2680,528 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5" s="23">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="47">
-        <v>244183</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="46" t="s">
+      <c r="C6" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A9" s="23">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A11" s="23">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="48" t="s">
-        <v>93</v>
+      <c r="D11" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A13" s="23">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A15" s="23">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A17" s="23">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A19" s="23">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A21" s="23">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="24"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A23" s="23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="25">
+        <v>244184</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>